<commit_message>
Need to reset LibXmlLoaderOptions before opening the test file
</commit_message>
<xml_diff>
--- a/tests/data/Worksheet/namedRangeTest.xlsx
+++ b/tests/data/Worksheet/namedRangeTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Worksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909D5137-DAB5-40C8-BE6D-DB1039CEA739}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD793012-2257-4B4A-9592-7B8B417E9AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3908" yWindow="1837" windowWidth="21599" windowHeight="13238" xr2:uid="{56818D25-0CED-47DD-BA6D-241CA815C284}"/>
   </bookViews>

</xml_diff>

<commit_message>
Additional tests for both happy and unhappy path
</commit_message>
<xml_diff>
--- a/tests/data/Worksheet/namedRangeTest.xlsx
+++ b/tests/data/Worksheet/namedRangeTest.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Worksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD793012-2257-4B4A-9592-7B8B417E9AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6A46F2-25C6-418A-BD18-EB5EC44F7ABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3908" yWindow="1837" windowWidth="21599" windowHeight="13238" xr2:uid="{56818D25-0CED-47DD-BA6D-241CA815C284}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Calculation" localSheetId="1">SUM(Sheet2!$A$1:$C$1)/SUM(Sheet2!$A$3/Sheet2!$C$3)</definedName>
     <definedName name="GREETING">Sheet1!$B$2</definedName>
     <definedName name="Range1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="Result" localSheetId="1">Sheet2!$E$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -428,4 +431,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6E482F-2A06-4E20-B9F5-EDFDFA91EFF7}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <f>Calculation</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cellExists() and getCell() methods should support UTF-8 named cells
</commit_message>
<xml_diff>
--- a/tests/data/Worksheet/namedRangeTest.xlsx
+++ b/tests/data/Worksheet/namedRangeTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25522"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Worksheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PhpSpreadsheet\tests\data\Worksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6A46F2-25C6-418A-BD18-EB5EC44F7ABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE3DCC-3B8C-4692-A791-0E90730C966F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3908" yWindow="1837" windowWidth="21599" windowHeight="13238" xr2:uid="{56818D25-0CED-47DD-BA6D-241CA815C284}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{56818D25-0CED-47DD-BA6D-241CA815C284}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,20 +21,35 @@
     <definedName name="GREETING">Sheet1!$B$2</definedName>
     <definedName name="Range1">Sheet1!$A$1:$C$1</definedName>
     <definedName name="Result" localSheetId="1">Sheet2!$E$1</definedName>
+    <definedName name="Χαιρετισμός">Sheet1!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>नमस्ते</t>
   </si>
 </sst>
 </file>
@@ -389,13 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80407197-2FF0-4472-BCE7-7844BA72F8F9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -406,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -417,7 +434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>7</v>
       </c>
@@ -426,6 +443,11 @@
       </c>
       <c r="C3" s="1">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -441,9 +463,9 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>9</v>
       </c>
@@ -458,7 +480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -469,7 +491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>

</xml_diff>